<commit_message>
Estamos hasta la callampa
</commit_message>
<xml_diff>
--- a/Opti/Datos/Demanda_comida.xlsx
+++ b/Opti/Datos/Demanda_comida.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/gaalfaro_uc_cl/Documents/Proyecto OPTI/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/nico_lavandero2004_uc_cl/Documents/Opti/Progra/Opti/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F557ABD-FF0F-48DC-98DA-3599A26551B3}"/>
+  <xr:revisionPtr revIDLastSave="353" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BEC3B3-4BF2-4318-AEBB-71EAC02B1E46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region 16" sheetId="10" r:id="rId1"/>
@@ -131,6 +131,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,18 +454,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87504A2-056E-48C9-93E9-E5D188B0A148}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,180 +476,218 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>7161.5249999999996</v>
+        <v>10230.75</v>
       </c>
       <c r="C2" s="4">
-        <v>35807.625</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51153.75</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>10230.75</v>
+        <v>33976.5</v>
       </c>
       <c r="C3" s="4">
-        <v>51153.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169882.5</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>33976.5</v>
+        <v>16988.25</v>
       </c>
       <c r="C4" s="4">
-        <v>169882.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84941.25</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>16988.25</v>
+        <v>23133</v>
       </c>
       <c r="C5" s="4">
-        <v>84941.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115665</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>23133</v>
+        <v>47292</v>
       </c>
       <c r="C6" s="4">
-        <v>115665</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>236460</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>47292</v>
+        <v>36400.5</v>
       </c>
       <c r="C7" s="4">
-        <v>236460</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>182002.5</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>141220.5</v>
+        <v>51846</v>
       </c>
       <c r="C8" s="4">
-        <v>706102.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259230</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>36400.5</v>
+        <v>49109.25</v>
       </c>
       <c r="C9" s="4">
-        <v>182002.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>245546.25</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>51846</v>
+        <v>31101</v>
       </c>
       <c r="C10" s="4">
         <v>259230</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>29856.75</v>
+      </c>
+      <c r="C11" s="4">
+        <v>149283.75</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4385.25</v>
+      </c>
+      <c r="C12" s="4">
+        <v>21926.25</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6708.75</v>
+      </c>
+      <c r="C13" s="4">
+        <v>33543.75</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>141220.5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>706102.5</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15780.75</v>
+      </c>
+      <c r="C15" s="4">
+        <v>78903.75</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7161.5249999999996</v>
+      </c>
+      <c r="C16" s="4">
+        <v>35807.625</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B17" s="2">
         <v>19631.25</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C17" s="4">
         <v>98156.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2">
-        <v>49109.25</v>
-      </c>
-      <c r="C12" s="4">
-        <v>245546.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2">
-        <v>31101</v>
-      </c>
-      <c r="C13" s="4">
-        <v>155505</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
-        <v>15780.75</v>
-      </c>
-      <c r="C14" s="4">
-        <v>78903.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2">
-        <v>29856.75</v>
-      </c>
-      <c r="C15" s="4">
-        <v>149283.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4385.25</v>
-      </c>
-      <c r="C16" s="4">
-        <v>21926.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>12</v>
-      </c>
-      <c r="B17" s="2">
-        <v>6708.75</v>
-      </c>
-      <c r="C17" s="4">
-        <v>33543.75</v>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f>SUM(B2:B17)</f>
+        <v>524822.02500000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>